<commit_message>
corrected line numbers and MAX1932 package
</commit_message>
<xml_diff>
--- a/cosmicpi_1.6.xlsx
+++ b/cosmicpi_1.6.xlsx
@@ -16,7 +16,7 @@
     <sheet name="cosmicpi_1.6" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="cosmicpi_1.6" localSheetId="0">Sheet1!$A$1:$N$63</definedName>
+    <definedName name="cosmicpi_1.6" localSheetId="0">Sheet1!$A$1:$N$62</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="511" uniqueCount="453">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="507" uniqueCount="451">
   <si>
     <t>Id;"Designator";"Package";"Quantity";"Designation";"Supplier and ref";</t>
   </si>
@@ -682,12 +682,6 @@
     <t>R_0603_1608Metric</t>
   </si>
   <si>
-    <t>H5,H6,H2,H4,H3,H1</t>
-  </si>
-  <si>
-    <t>MountingHole_3.7mm</t>
-  </si>
-  <si>
     <t>IND_744232090</t>
   </si>
   <si>
@@ -916,9 +910,6 @@
     <t>U17,U18</t>
   </si>
   <si>
-    <t>QFN-16-1EP_4x4mm_P0.65mm_EP2.5x2.5mm</t>
-  </si>
-  <si>
     <t>MAX1932</t>
   </si>
   <si>
@@ -1406,6 +1397,9 @@
   </si>
   <si>
     <t>R50,R51,R45,R44,R43,R42</t>
+  </si>
+  <si>
+    <t>21-0136I_T1233-3</t>
   </si>
 </sst>
 </file>
@@ -2244,10 +2238,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,31 +2267,31 @@
         <v>203</v>
       </c>
       <c r="C1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D1" t="s">
         <v>205</v>
       </c>
       <c r="E1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G1" t="s">
         <v>204</v>
       </c>
       <c r="H1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="I1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="J1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="K1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2308,13 +2302,13 @@
         <v>206</v>
       </c>
       <c r="C2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D2">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G2" t="s">
         <v>207</v>
@@ -2325,19 +2319,20 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
+        <f>SUM(A2+1)</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>209</v>
       </c>
       <c r="C3" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="G3" t="s">
         <v>210</v>
@@ -2349,24 +2344,31 @@
         <v>0.01</v>
       </c>
       <c r="K3" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
+        <f t="shared" ref="A4:A62" si="0">SUM(A3+1)</f>
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="C4" t="s">
+        <v>352</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>354</v>
+      </c>
+      <c r="F4" t="s">
+        <v>355</v>
+      </c>
+      <c r="G4" t="s">
         <v>211</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>354</v>
-      </c>
-      <c r="G4" t="s">
-        <v>212</v>
       </c>
       <c r="H4" t="s">
         <v>212</v>
@@ -2374,214 +2376,221 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>449</v>
+      <c r="B5" t="s">
+        <v>213</v>
       </c>
       <c r="C5" t="s">
-        <v>355</v>
-      </c>
-      <c r="D5" s="5">
-        <v>2</v>
+        <v>353</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>357</v>
-      </c>
-      <c r="F5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>215</v>
-      </c>
-      <c r="C6" t="s">
-        <v>356</v>
+        <v>216</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>357</v>
       </c>
       <c r="D6">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
-        <v>359</v>
-      </c>
       <c r="G6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>218</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>360</v>
+        <v>219</v>
+      </c>
+      <c r="C7" t="s">
+        <v>358</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>221</v>
-      </c>
-      <c r="C8" t="s">
-        <v>361</v>
+        <v>222</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>402</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>224</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>405</v>
+        <v>225</v>
+      </c>
+      <c r="C9" t="s">
+        <v>384</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H9" t="s">
-        <v>226</v>
+        <v>227</v>
+      </c>
+      <c r="I9" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C10" t="s">
+        <v>386</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>387</v>
       </c>
-      <c r="D10">
-        <v>30</v>
-      </c>
       <c r="G10" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H10" t="s">
         <v>229</v>
       </c>
       <c r="I10" t="s">
-        <v>386</v>
+        <v>385</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>230</v>
       </c>
       <c r="C11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>390</v>
+        <v>6</v>
       </c>
       <c r="G11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H11" t="s">
         <v>231</v>
       </c>
       <c r="I11" t="s">
-        <v>388</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0.2</v>
+        <v>383</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>232</v>
       </c>
       <c r="C12" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H12" t="s">
         <v>233</v>
       </c>
       <c r="I12" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>13</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>234</v>
       </c>
       <c r="C13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G13" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H13" t="s">
         <v>235</v>
       </c>
       <c r="I13" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>14</v>
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>236</v>
@@ -2590,49 +2599,57 @@
         <v>393</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H14" t="s">
         <v>237</v>
       </c>
       <c r="I14" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>15</v>
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>238</v>
       </c>
-      <c r="C15" t="s">
-        <v>396</v>
+      <c r="C15" s="3" t="s">
+        <v>394</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
+      <c r="E15" t="s">
+        <v>395</v>
+      </c>
       <c r="G15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H15" t="s">
         <v>239</v>
       </c>
       <c r="I15" t="s">
-        <v>395</v>
+        <v>396</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.05</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>16</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>240</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" t="s">
         <v>397</v>
       </c>
       <c r="D16">
@@ -2642,13 +2659,13 @@
         <v>398</v>
       </c>
       <c r="G16" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H16" t="s">
         <v>241</v>
       </c>
       <c r="I16" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
       <c r="J16" s="1">
         <v>0.05</v>
@@ -2656,261 +2673,266 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>17</v>
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>242</v>
       </c>
       <c r="C17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H17" t="s">
         <v>243</v>
       </c>
       <c r="I17" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="J17" s="1">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>18</v>
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>244</v>
       </c>
       <c r="C18" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D18">
         <v>2</v>
       </c>
-      <c r="E18" t="s">
-        <v>403</v>
-      </c>
       <c r="G18" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
       <c r="H18" t="s">
-        <v>245</v>
-      </c>
-      <c r="I18" t="s">
-        <v>386</v>
-      </c>
-      <c r="J18" s="1">
-        <v>0.1</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>19</v>
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>246</v>
       </c>
-      <c r="C19" t="s">
-        <v>404</v>
-      </c>
       <c r="D19">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>351</v>
       </c>
       <c r="G19" t="s">
         <v>247</v>
       </c>
       <c r="H19" t="s">
-        <v>229</v>
+        <v>248</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>248</v>
+        <v>249</v>
+      </c>
+      <c r="C20" t="s">
+        <v>403</v>
       </c>
       <c r="D20">
-        <v>4</v>
-      </c>
-      <c r="F20" t="s">
-        <v>354</v>
+        <v>15</v>
       </c>
       <c r="G20" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H20" t="s">
         <v>250</v>
       </c>
+      <c r="I20" t="s">
+        <v>391</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>21</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>251</v>
       </c>
       <c r="C21" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D21">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H21" t="s">
         <v>252</v>
       </c>
       <c r="I21" t="s">
-        <v>394</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.2</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>22</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>253</v>
       </c>
       <c r="C22" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
+      <c r="E22" t="s">
+        <v>408</v>
+      </c>
       <c r="G22" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="H22" t="s">
-        <v>254</v>
+        <v>409</v>
       </c>
       <c r="I22" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="J22" s="1">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>23</v>
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>255</v>
-      </c>
-      <c r="C23" t="s">
-        <v>410</v>
+        <v>254</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>359</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="E23" t="s">
-        <v>411</v>
-      </c>
       <c r="G23" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="H23" t="s">
-        <v>412</v>
-      </c>
-      <c r="I23" t="s">
-        <v>399</v>
-      </c>
-      <c r="J23" s="1">
-        <v>0.1</v>
+        <v>256</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>24</v>
+        <f t="shared" si="0"/>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>256</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>362</v>
+        <v>257</v>
+      </c>
+      <c r="C24" t="s">
+        <v>410</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
+      <c r="E24" t="s">
+        <v>411</v>
+      </c>
       <c r="G24" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H24" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>25</v>
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C25" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G25" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H25" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>26</v>
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C26" t="s">
-        <v>415</v>
+        <v>360</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
-      <c r="E26" t="s">
-        <v>416</v>
-      </c>
       <c r="G26" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H26" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>27</v>
-      </c>
-      <c r="B27" t="s">
-        <v>265</v>
-      </c>
-      <c r="C27" t="s">
-        <v>363</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D27" s="5">
+        <v>2</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>361</v>
       </c>
       <c r="G27" t="s">
         <v>266</v>
@@ -2921,48 +2943,47 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>28</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="D28" s="5">
-        <v>2</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>364</v>
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>268</v>
+      </c>
+      <c r="C28" t="s">
+        <v>362</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>270</v>
+      </c>
+      <c r="F28" t="s">
+        <v>363</v>
       </c>
       <c r="G28" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H28" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C29" t="s">
-        <v>365</v>
+        <v>415</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
-      <c r="E29" t="s">
-        <v>272</v>
-      </c>
-      <c r="F29" t="s">
-        <v>366</v>
-      </c>
       <c r="G29" t="s">
-        <v>271</v>
+        <v>414</v>
       </c>
       <c r="H29" t="s">
         <v>272</v>
@@ -2970,125 +2991,131 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>31</v>
+        <f t="shared" si="0"/>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>273</v>
       </c>
       <c r="C30" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>417</v>
+        <v>274</v>
       </c>
       <c r="H30" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>32</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C31" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
+      <c r="F31" t="s">
+        <v>419</v>
+      </c>
       <c r="G31" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H31" t="s">
-        <v>277</v>
+        <v>417</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>33</v>
+        <f t="shared" si="0"/>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>277</v>
+      </c>
+      <c r="C32" t="s">
+        <v>420</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
         <v>278</v>
       </c>
-      <c r="C32" t="s">
-        <v>421</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="F32" t="s">
-        <v>422</v>
-      </c>
-      <c r="G32" t="s">
-        <v>276</v>
-      </c>
       <c r="H32" t="s">
-        <v>420</v>
+        <v>279</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>34</v>
+        <f t="shared" si="0"/>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C33" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="E33" t="s">
+        <v>422</v>
       </c>
       <c r="G33" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H33" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>35</v>
+        <f t="shared" si="0"/>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C34" t="s">
-        <v>424</v>
+        <v>367</v>
       </c>
       <c r="D34">
-        <v>4</v>
-      </c>
-      <c r="E34" t="s">
-        <v>425</v>
+        <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H34" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>36</v>
+        <f t="shared" si="0"/>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C35" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G35" t="s">
-        <v>286</v>
+        <v>450</v>
       </c>
       <c r="H35" t="s">
         <v>287</v>
@@ -3096,16 +3123,17 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>37</v>
+        <f t="shared" si="0"/>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>288</v>
       </c>
       <c r="C36" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G36" t="s">
         <v>289</v>
@@ -3116,13 +3144,14 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>38</v>
+        <f t="shared" si="0"/>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>291</v>
       </c>
       <c r="C37" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -3136,13 +3165,14 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>39</v>
+        <f t="shared" si="0"/>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>294</v>
       </c>
       <c r="C38" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -3156,17 +3186,21 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>297</v>
       </c>
       <c r="C39" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
+      <c r="E39" t="s">
+        <v>365</v>
+      </c>
       <c r="G39" t="s">
         <v>298</v>
       </c>
@@ -3176,19 +3210,20 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>41</v>
+        <f t="shared" si="0"/>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>300</v>
       </c>
       <c r="C40" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G40" t="s">
         <v>301</v>
@@ -3199,19 +3234,17 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>42</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>303</v>
       </c>
       <c r="C41" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" t="s">
-        <v>375</v>
+        <v>3</v>
       </c>
       <c r="G41" t="s">
         <v>304</v>
@@ -3222,59 +3255,65 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>43</v>
+        <f t="shared" si="0"/>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>306</v>
       </c>
       <c r="C42" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D42">
         <v>3</v>
       </c>
       <c r="G42" t="s">
+        <v>304</v>
+      </c>
+      <c r="H42" t="s">
         <v>307</v>
-      </c>
-      <c r="H42" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>44</v>
+        <f t="shared" si="0"/>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>308</v>
+      </c>
+      <c r="C43" t="s">
+        <v>375</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="G43" t="s">
+        <v>304</v>
+      </c>
+      <c r="H43" t="s">
         <v>309</v>
-      </c>
-      <c r="C43" t="s">
-        <v>377</v>
-      </c>
-      <c r="D43">
-        <v>3</v>
-      </c>
-      <c r="G43" t="s">
-        <v>307</v>
-      </c>
-      <c r="H43" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>45</v>
+        <f t="shared" si="0"/>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C44" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
+      <c r="E44" t="s">
+        <v>377</v>
+      </c>
       <c r="G44" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="H44" t="s">
         <v>312</v>
@@ -3282,45 +3321,47 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>46</v>
+        <f t="shared" si="0"/>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>313</v>
       </c>
       <c r="C45" t="s">
-        <v>379</v>
+        <v>314</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G45" t="s">
+        <v>207</v>
+      </c>
+      <c r="H45" t="s">
         <v>314</v>
-      </c>
-      <c r="H45" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>47</v>
+        <f t="shared" si="0"/>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C46" t="s">
-        <v>317</v>
+        <v>379</v>
       </c>
       <c r="D46">
         <v>2</v>
       </c>
       <c r="E46" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G46" t="s">
-        <v>207</v>
+        <v>316</v>
       </c>
       <c r="H46" t="s">
         <v>317</v>
@@ -3328,192 +3369,203 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>48</v>
+        <f t="shared" si="0"/>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>318</v>
       </c>
       <c r="C47" t="s">
-        <v>382</v>
+        <v>425</v>
       </c>
       <c r="D47">
         <v>2</v>
       </c>
-      <c r="E47" t="s">
-        <v>383</v>
-      </c>
       <c r="G47" t="s">
+        <v>210</v>
+      </c>
+      <c r="H47" t="s">
         <v>319</v>
       </c>
-      <c r="H47" t="s">
-        <v>320</v>
+      <c r="J47" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K47" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>49</v>
+        <f t="shared" si="0"/>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>321</v>
-      </c>
-      <c r="C48" t="s">
-        <v>428</v>
+        <v>320</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>426</v>
       </c>
       <c r="D48">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="G48" t="s">
         <v>210</v>
       </c>
       <c r="H48" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J48" s="1">
         <v>0.01</v>
       </c>
       <c r="K48" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>323</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>429</v>
+        <v>322</v>
+      </c>
+      <c r="C49" t="s">
+        <v>428</v>
       </c>
       <c r="D49">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="G49" t="s">
         <v>210</v>
       </c>
       <c r="H49" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J49" s="1">
         <v>0.01</v>
       </c>
       <c r="K49" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>51</v>
+        <f t="shared" si="0"/>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>325</v>
+        <v>449</v>
       </c>
       <c r="C50" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G50" t="s">
         <v>210</v>
       </c>
       <c r="H50" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="J50" s="1">
         <v>0.01</v>
       </c>
       <c r="K50" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>52</v>
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>452</v>
+        <v>325</v>
       </c>
       <c r="C51" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D51">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G51" t="s">
         <v>210</v>
       </c>
       <c r="H51" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J51" s="1">
         <v>0.01</v>
       </c>
       <c r="K51" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>53</v>
+        <f t="shared" si="0"/>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C52" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D52">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G52" t="s">
         <v>210</v>
       </c>
-      <c r="H52" t="s">
-        <v>329</v>
+      <c r="H52">
+        <v>100</v>
       </c>
       <c r="J52" s="1">
         <v>0.01</v>
       </c>
       <c r="K52" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>54</v>
+        <f t="shared" si="0"/>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C53" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D53">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G53" t="s">
         <v>210</v>
       </c>
-      <c r="H53">
-        <v>100</v>
+      <c r="H53" t="s">
+        <v>329</v>
       </c>
       <c r="J53" s="1">
         <v>0.01</v>
       </c>
       <c r="K53" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>55</v>
+        <f t="shared" si="0"/>
+        <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C54" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D54">
         <v>4</v>
@@ -3521,80 +3573,83 @@
       <c r="G54" t="s">
         <v>210</v>
       </c>
-      <c r="H54" t="s">
-        <v>332</v>
+      <c r="H54">
+        <v>300</v>
       </c>
       <c r="J54" s="1">
         <v>0.01</v>
       </c>
       <c r="K54" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>57</v>
+        <f t="shared" si="0"/>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C55" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D55">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="E55" t="s">
+        <v>435</v>
       </c>
       <c r="G55" t="s">
         <v>210</v>
       </c>
-      <c r="H55">
-        <v>300</v>
+      <c r="H55" t="s">
+        <v>332</v>
       </c>
       <c r="J55" s="1">
         <v>0.01</v>
       </c>
       <c r="K55" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>58</v>
+        <f t="shared" si="0"/>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C56" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D56">
         <v>2</v>
       </c>
-      <c r="E56" t="s">
-        <v>438</v>
-      </c>
       <c r="G56" t="s">
         <v>210</v>
       </c>
       <c r="H56" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="J56" s="1">
         <v>0.01</v>
       </c>
       <c r="K56" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>59</v>
+        <f t="shared" si="0"/>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C57" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D57">
         <v>2</v>
@@ -3602,176 +3657,155 @@
       <c r="G57" t="s">
         <v>210</v>
       </c>
-      <c r="H57" t="s">
-        <v>337</v>
+      <c r="H57">
+        <v>806</v>
       </c>
       <c r="J57" s="1">
         <v>0.01</v>
       </c>
       <c r="K57" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>60</v>
+        <f t="shared" si="0"/>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C58" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="D58">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="E58" t="s">
+        <v>438</v>
       </c>
       <c r="G58" t="s">
         <v>210</v>
       </c>
-      <c r="H58">
-        <v>806</v>
+      <c r="H58" t="s">
+        <v>337</v>
       </c>
       <c r="J58" s="1">
         <v>0.01</v>
       </c>
       <c r="K58" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>61</v>
+        <f t="shared" si="0"/>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C59" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="D59">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G59" t="s">
         <v>210</v>
       </c>
-      <c r="H59" t="s">
-        <v>340</v>
+      <c r="H59">
+        <v>10</v>
       </c>
       <c r="J59" s="1">
         <v>0.01</v>
       </c>
       <c r="K59" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>62</v>
+        <f t="shared" si="0"/>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C60" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="G60" t="s">
         <v>210</v>
       </c>
-      <c r="H60">
-        <v>10</v>
+      <c r="H60" t="s">
+        <v>340</v>
       </c>
       <c r="J60" s="1">
         <v>0.01</v>
       </c>
       <c r="K60" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>63</v>
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C61" t="s">
-        <v>430</v>
+        <v>442</v>
       </c>
       <c r="D61">
-        <v>2</v>
-      </c>
-      <c r="E61" t="s">
-        <v>444</v>
+        <v>1</v>
       </c>
       <c r="G61" t="s">
         <v>210</v>
       </c>
       <c r="H61" t="s">
-        <v>343</v>
-      </c>
-      <c r="J61" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="K61" t="s">
-        <v>427</v>
+        <v>342</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>64</v>
-      </c>
-      <c r="B62" t="s">
-        <v>344</v>
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>445</v>
       </c>
       <c r="C62" t="s">
-        <v>445</v>
-      </c>
-      <c r="D62">
-        <v>1</v>
+        <v>443</v>
+      </c>
+      <c r="D62" s="5">
+        <v>5</v>
+      </c>
+      <c r="E62" t="s">
+        <v>444</v>
       </c>
       <c r="G62" t="s">
         <v>210</v>
       </c>
-      <c r="H62" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>65</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="C63" t="s">
-        <v>446</v>
-      </c>
-      <c r="D63" s="5">
-        <v>5</v>
-      </c>
-      <c r="E63" t="s">
-        <v>447</v>
-      </c>
-      <c r="G63" t="s">
-        <v>210</v>
-      </c>
-      <c r="H63">
+      <c r="H62">
         <v>20</v>
       </c>
-      <c r="J63" s="1">
+      <c r="J62" s="1">
         <v>0.01</v>
       </c>
-      <c r="K63" t="s">
-        <v>427</v>
+      <c r="K62" t="s">
+        <v>424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated board size to fit in housing
</commit_message>
<xml_diff>
--- a/cosmicpi_1.6.xlsx
+++ b/cosmicpi_1.6.xlsx
@@ -2238,16 +2238,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="B11:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="2" max="2" width="110.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
@@ -3809,8 +3812,9 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="8" scale="65" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changed router width from .15 to .8mm
feedback from Newbury Electronics who are manufacturing our first batch.
</commit_message>
<xml_diff>
--- a/cosmicpi_1.6.xlsx
+++ b/cosmicpi_1.6.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="507" uniqueCount="451">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="506" uniqueCount="450">
   <si>
     <t>Id;"Designator";"Package";"Quantity";"Designation";"Supplier and ref";</t>
   </si>
@@ -1103,9 +1103,6 @@
   </si>
   <si>
     <t>DNP</t>
-  </si>
-  <si>
-    <t>WE-CNSW_1812</t>
   </si>
   <si>
     <t xml:space="preserve">800-80-002-20-001101 </t>
@@ -2244,7 +2241,7 @@
   <dimension ref="A1:K62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="B11:E15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2294,7 +2291,7 @@
         <v>348</v>
       </c>
       <c r="K1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2329,13 +2326,13 @@
         <v>209</v>
       </c>
       <c r="C3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G3" t="s">
         <v>210</v>
@@ -2347,7 +2344,7 @@
         <v>0.01</v>
       </c>
       <c r="K3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2356,19 +2353,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="C4" t="s">
-        <v>352</v>
+        <v>445</v>
+      </c>
+      <c r="C4">
+        <v>744235220</v>
       </c>
       <c r="D4" s="5">
         <v>2</v>
       </c>
       <c r="E4" t="s">
+        <v>353</v>
+      </c>
+      <c r="F4" t="s">
         <v>354</v>
-      </c>
-      <c r="F4" t="s">
-        <v>355</v>
       </c>
       <c r="G4" t="s">
         <v>211</v>
@@ -2386,13 +2383,13 @@
         <v>213</v>
       </c>
       <c r="C5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G5" t="s">
         <v>214</v>
@@ -2410,7 +2407,7 @@
         <v>216</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -2431,7 +2428,7 @@
         <v>219</v>
       </c>
       <c r="C7" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -2452,7 +2449,7 @@
         <v>222</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2473,7 +2470,7 @@
         <v>225</v>
       </c>
       <c r="C9" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D9">
         <v>30</v>
@@ -2485,7 +2482,7 @@
         <v>227</v>
       </c>
       <c r="I9" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2497,13 +2494,13 @@
         <v>228</v>
       </c>
       <c r="C10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G10" t="s">
         <v>226</v>
@@ -2512,7 +2509,7 @@
         <v>229</v>
       </c>
       <c r="I10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J10" s="1">
         <v>0.2</v>
@@ -2527,7 +2524,7 @@
         <v>230</v>
       </c>
       <c r="C11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D11">
         <v>6</v>
@@ -2539,7 +2536,7 @@
         <v>231</v>
       </c>
       <c r="I11" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2551,7 +2548,7 @@
         <v>232</v>
       </c>
       <c r="C12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -2563,7 +2560,7 @@
         <v>233</v>
       </c>
       <c r="I12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2575,7 +2572,7 @@
         <v>234</v>
       </c>
       <c r="C13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -2587,7 +2584,7 @@
         <v>235</v>
       </c>
       <c r="I13" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2599,7 +2596,7 @@
         <v>236</v>
       </c>
       <c r="C14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -2611,7 +2608,7 @@
         <v>237</v>
       </c>
       <c r="I14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2623,13 +2620,13 @@
         <v>238</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G15" t="s">
         <v>226</v>
@@ -2638,7 +2635,7 @@
         <v>239</v>
       </c>
       <c r="I15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J15" s="1">
         <v>0.05</v>
@@ -2653,13 +2650,13 @@
         <v>240</v>
       </c>
       <c r="C16" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G16" t="s">
         <v>226</v>
@@ -2668,7 +2665,7 @@
         <v>241</v>
       </c>
       <c r="I16" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J16" s="1">
         <v>0.05</v>
@@ -2683,13 +2680,13 @@
         <v>242</v>
       </c>
       <c r="C17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G17" t="s">
         <v>226</v>
@@ -2698,7 +2695,7 @@
         <v>243</v>
       </c>
       <c r="I17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J17" s="1">
         <v>0.1</v>
@@ -2713,7 +2710,7 @@
         <v>244</v>
       </c>
       <c r="C18" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -2755,7 +2752,7 @@
         <v>249</v>
       </c>
       <c r="C20" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D20">
         <v>15</v>
@@ -2767,10 +2764,10 @@
         <v>250</v>
       </c>
       <c r="I20" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2782,7 +2779,7 @@
         <v>251</v>
       </c>
       <c r="C21" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -2794,7 +2791,7 @@
         <v>252</v>
       </c>
       <c r="I21" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J21" s="1">
         <v>0.2</v>
@@ -2809,22 +2806,22 @@
         <v>253</v>
       </c>
       <c r="C22" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G22" t="s">
         <v>245</v>
       </c>
       <c r="H22" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="I22" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J22" s="1">
         <v>0.1</v>
@@ -2839,7 +2836,7 @@
         <v>254</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -2860,13 +2857,13 @@
         <v>257</v>
       </c>
       <c r="C24" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G24" t="s">
         <v>258</v>
@@ -2884,13 +2881,13 @@
         <v>260</v>
       </c>
       <c r="C25" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G25" t="s">
         <v>261</v>
@@ -2908,7 +2905,7 @@
         <v>263</v>
       </c>
       <c r="C26" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -2926,16 +2923,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>447</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>448</v>
       </c>
       <c r="D27" s="5">
         <v>2</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G27" t="s">
         <v>266</v>
@@ -2953,7 +2950,7 @@
         <v>268</v>
       </c>
       <c r="C28" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -2962,7 +2959,7 @@
         <v>270</v>
       </c>
       <c r="F28" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G28" t="s">
         <v>269</v>
@@ -2980,13 +2977,13 @@
         <v>271</v>
       </c>
       <c r="C29" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H29" t="s">
         <v>272</v>
@@ -3001,7 +2998,7 @@
         <v>273</v>
       </c>
       <c r="C30" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -3022,19 +3019,19 @@
         <v>276</v>
       </c>
       <c r="C31" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G31" t="s">
         <v>274</v>
       </c>
       <c r="H31" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -3046,7 +3043,7 @@
         <v>277</v>
       </c>
       <c r="C32" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -3067,13 +3064,13 @@
         <v>280</v>
       </c>
       <c r="C33" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D33">
         <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G33" t="s">
         <v>281</v>
@@ -3091,7 +3088,7 @@
         <v>283</v>
       </c>
       <c r="C34" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -3112,13 +3109,13 @@
         <v>286</v>
       </c>
       <c r="C35" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D35">
         <v>2</v>
       </c>
       <c r="G35" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H35" t="s">
         <v>287</v>
@@ -3133,7 +3130,7 @@
         <v>288</v>
       </c>
       <c r="C36" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -3154,7 +3151,7 @@
         <v>291</v>
       </c>
       <c r="C37" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -3175,7 +3172,7 @@
         <v>294</v>
       </c>
       <c r="C38" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -3196,13 +3193,13 @@
         <v>297</v>
       </c>
       <c r="C39" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G39" t="s">
         <v>298</v>
@@ -3220,13 +3217,13 @@
         <v>300</v>
       </c>
       <c r="C40" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G40" t="s">
         <v>301</v>
@@ -3244,7 +3241,7 @@
         <v>303</v>
       </c>
       <c r="C41" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D41">
         <v>3</v>
@@ -3265,7 +3262,7 @@
         <v>306</v>
       </c>
       <c r="C42" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D42">
         <v>3</v>
@@ -3286,7 +3283,7 @@
         <v>308</v>
       </c>
       <c r="C43" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -3307,13 +3304,13 @@
         <v>310</v>
       </c>
       <c r="C44" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G44" t="s">
         <v>311</v>
@@ -3337,7 +3334,7 @@
         <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G45" t="s">
         <v>207</v>
@@ -3355,13 +3352,13 @@
         <v>315</v>
       </c>
       <c r="C46" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D46">
         <v>2</v>
       </c>
       <c r="E46" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G46" t="s">
         <v>316</v>
@@ -3379,7 +3376,7 @@
         <v>318</v>
       </c>
       <c r="C47" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D47">
         <v>2</v>
@@ -3394,7 +3391,7 @@
         <v>0.01</v>
       </c>
       <c r="K47" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -3406,7 +3403,7 @@
         <v>320</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D48">
         <v>21</v>
@@ -3421,7 +3418,7 @@
         <v>0.01</v>
       </c>
       <c r="K48" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -3433,7 +3430,7 @@
         <v>322</v>
       </c>
       <c r="C49" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -3448,7 +3445,7 @@
         <v>0.01</v>
       </c>
       <c r="K49" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -3457,10 +3454,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C50" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D50">
         <v>6</v>
@@ -3475,7 +3472,7 @@
         <v>0.01</v>
       </c>
       <c r="K50" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -3487,7 +3484,7 @@
         <v>325</v>
       </c>
       <c r="C51" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D51">
         <v>2</v>
@@ -3502,7 +3499,7 @@
         <v>0.01</v>
       </c>
       <c r="K51" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -3514,7 +3511,7 @@
         <v>327</v>
       </c>
       <c r="C52" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D52">
         <v>6</v>
@@ -3529,7 +3526,7 @@
         <v>0.01</v>
       </c>
       <c r="K52" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -3541,7 +3538,7 @@
         <v>328</v>
       </c>
       <c r="C53" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D53">
         <v>4</v>
@@ -3556,7 +3553,7 @@
         <v>0.01</v>
       </c>
       <c r="K53" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -3568,7 +3565,7 @@
         <v>330</v>
       </c>
       <c r="C54" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D54">
         <v>4</v>
@@ -3583,7 +3580,7 @@
         <v>0.01</v>
       </c>
       <c r="K54" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -3595,13 +3592,13 @@
         <v>331</v>
       </c>
       <c r="C55" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D55">
         <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G55" t="s">
         <v>210</v>
@@ -3613,7 +3610,7 @@
         <v>0.01</v>
       </c>
       <c r="K55" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -3625,7 +3622,7 @@
         <v>333</v>
       </c>
       <c r="C56" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D56">
         <v>2</v>
@@ -3640,7 +3637,7 @@
         <v>0.01</v>
       </c>
       <c r="K56" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -3652,7 +3649,7 @@
         <v>335</v>
       </c>
       <c r="C57" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D57">
         <v>2</v>
@@ -3667,7 +3664,7 @@
         <v>0.01</v>
       </c>
       <c r="K57" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -3679,13 +3676,13 @@
         <v>336</v>
       </c>
       <c r="C58" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D58">
         <v>7</v>
       </c>
       <c r="E58" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G58" t="s">
         <v>210</v>
@@ -3697,7 +3694,7 @@
         <v>0.01</v>
       </c>
       <c r="K58" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -3709,13 +3706,13 @@
         <v>338</v>
       </c>
       <c r="C59" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G59" t="s">
         <v>210</v>
@@ -3727,7 +3724,7 @@
         <v>0.01</v>
       </c>
       <c r="K59" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -3739,13 +3736,13 @@
         <v>339</v>
       </c>
       <c r="C60" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D60">
         <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G60" t="s">
         <v>210</v>
@@ -3757,7 +3754,7 @@
         <v>0.01</v>
       </c>
       <c r="K60" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -3769,7 +3766,7 @@
         <v>341</v>
       </c>
       <c r="C61" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -3787,16 +3784,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C62" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D62" s="5">
         <v>5</v>
       </c>
       <c r="E62" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G62" t="s">
         <v>210</v>
@@ -3808,7 +3805,7 @@
         <v>0.01</v>
       </c>
       <c r="K62" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>